<commit_message>
try just the last output from rnn - no better
</commit_message>
<xml_diff>
--- a/hw2sent/good_models.xlsx
+++ b/hw2sent/good_models.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
   <si>
     <t>Assignment 2 best results</t>
   </si>
@@ -106,9 +106,6 @@
   </si>
   <si>
     <t>L2 beta</t>
-  </si>
-  <si>
-    <t>20171004-214746</t>
   </si>
 </sst>
 </file>
@@ -711,9 +708,6 @@
       <c r="J9" s="2">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="K9" s="3" t="s">
-        <v>29</v>
-      </c>
       <c r="L9" s="2">
         <v>50000</v>
       </c>

</xml_diff>